<commit_message>
Add more  verified accuracy functions
</commit_message>
<xml_diff>
--- a/verification/opt_results/exp19.xlsx
+++ b/verification/opt_results/exp19.xlsx
@@ -489,13 +489,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>235</v>
       </c>
       <c r="F2" t="n">
-        <v>97</v>
+        <v>231</v>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>

</xml_diff>